<commit_message>
Not done yet, but trying to improve robustness of the regressor so final outputs are insensitive to initial guess
</commit_message>
<xml_diff>
--- a/case2_Glu-Fru/_FG_ISOTHERMS_ANALYSED.xlsx
+++ b/case2_Glu-Fru/_FG_ISOTHERMS_ANALYSED.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case2_Glu-Fru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8615791D-DC6D-4D70-8E76-7A990C430F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584596E5-9231-4B1B-92ED-93B743AC858D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{EA7960EC-E79E-451C-8537-779F67CA9E08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EA7960EC-E79E-451C-8537-779F67CA9E08}"/>
   </bookViews>
   <sheets>
     <sheet name="GLUCOSE (2)" sheetId="5" r:id="rId1"/>
@@ -36,8 +36,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={15736140-9E9C-445F-BC03-F61B551C7F08}</author>
+  </authors>
+  <commentList>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{15736140-9E9C-445F-BC03-F61B551C7F08}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Just an estimate from UBK:
+https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={47062DED-F4B9-4D63-B1E0-DBB4945A7021}</author>
+  </authors>
+  <commentList>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{47062DED-F4B9-4D63-B1E0-DBB4945A7021}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Just an estimate from UBK:
+https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>R1</t>
   </si>
@@ -86,16 +126,36 @@
   <si>
     <t>Ce/Qe</t>
   </si>
+  <si>
+    <t>For Model</t>
+  </si>
+  <si>
+    <t>Ce (g/mL)</t>
+  </si>
+  <si>
+    <t>Qe (g/g_resin)</t>
+  </si>
+  <si>
+    <t>Qe(g/mL_resin</t>
+  </si>
+  <si>
+    <t>Resin Density (g_resin/mL_resin)</t>
+  </si>
+  <si>
+    <t>Qe(g/mL_resin)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +175,12 @@
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -329,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -483,6 +549,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2655,6 +2728,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Punabantu, N, Mr [28820169@sun.ac.za]" id="{02DB9639-B0EA-4BF2-BA53-BACC86B10F58}" userId="S::28820169@sun.ac.za::4361c9af-2042-4bd0-a173-bb9a66611d75" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2970,19 +3049,54 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B18" dT="2025-06-11T12:49:59.36" personId="{02DB9639-B0EA-4BF2-BA53-BACC86B10F58}" id="{15736140-9E9C-445F-BC03-F61B551C7F08}">
+    <text xml:space="preserve">Just an estimate from UBK:
+https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf
+</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3247326814</xltc2:checksum>
+        <xltc2:hyperlink startIndex="27" length="107" url="https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D19" dT="2025-06-11T12:49:59.36" personId="{02DB9639-B0EA-4BF2-BA53-BACC86B10F58}" id="{47062DED-F4B9-4D63-B1E0-DBB4945A7021}">
+    <text xml:space="preserve">Just an estimate from UBK:
+https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf
+</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3247326814</xltc2:checksum>
+        <xltc2:hyperlink startIndex="27" length="107" url="https://www.diaion.com/en/products/ion_exchange_resins/strongly_acidic_cation/data_sheet_ubk/pdf/ubk530.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4902D9D6-E2C9-4146-893E-01F7E3E9B95B}">
-  <dimension ref="B1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4902D9D6-E2C9-4146-893E-01F7E3E9B95B}">
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.109375" style="1"/>
-    <col min="6" max="6" width="12.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.109375" style="1"/>
     <col min="10" max="10" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -3152,7 +3266,7 @@
         <v>1.55</v>
       </c>
       <c r="G8" s="22">
-        <f t="shared" ref="G7:G12" si="4">B8-F8</f>
+        <f t="shared" ref="G8:G12" si="4">B8-F8</f>
         <v>1.57</v>
       </c>
       <c r="H8" s="23">
@@ -3258,7 +3372,7 @@
         <v>0.92</v>
       </c>
       <c r="H11" s="23">
-        <f t="shared" si="1"/>
+        <f>G11*$D$2/(1000*$D$3)</f>
         <v>3.0666666666666672E-3</v>
       </c>
       <c r="I11" s="31">
@@ -3304,24 +3418,155 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="65"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="63">
+        <f>F12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="64">
+        <f>H12</f>
+        <v>2.0333333333333332E-3</v>
+      </c>
+      <c r="G17" s="67">
+        <f>F17*$B$19</f>
+        <v>2.4806666666666666E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="63">
+        <f>F11/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="64">
+        <f>H11</f>
+        <v>3.0666666666666672E-3</v>
+      </c>
+      <c r="G18" s="67">
+        <f t="shared" ref="G18:G23" si="5">F18*$B$19</f>
+        <v>3.7413333333333339E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="66">
+        <v>1.22</v>
+      </c>
+      <c r="E19" s="63">
+        <f>F10/1000</f>
+        <v>7.3333333333333334E-4</v>
+      </c>
+      <c r="F19" s="64">
+        <f>H10</f>
+        <v>3.1555555555555551E-3</v>
+      </c>
+      <c r="G19" s="67">
+        <f t="shared" si="5"/>
+        <v>3.8497777777777771E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="63">
+        <f>F9/1000</f>
+        <v>1.0366666666666666E-3</v>
+      </c>
+      <c r="F20" s="64">
+        <f>H9</f>
+        <v>4.8777777777777778E-3</v>
+      </c>
+      <c r="G20" s="67">
+        <f t="shared" si="5"/>
+        <v>5.9508888888888884E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="63">
+        <f>F8/1000</f>
+        <v>1.5499999999999999E-3</v>
+      </c>
+      <c r="F21" s="64">
+        <f>H8</f>
+        <v>5.2333333333333338E-3</v>
+      </c>
+      <c r="G21" s="67">
+        <f t="shared" si="5"/>
+        <v>6.384666666666667E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="63">
+        <f>F7/1000</f>
+        <v>2.1366666666666669E-3</v>
+      </c>
+      <c r="F22" s="64">
+        <f>H7</f>
+        <v>7.9444444444444432E-3</v>
+      </c>
+      <c r="G22" s="67">
+        <f t="shared" si="5"/>
+        <v>9.6922222222222201E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="63">
+        <f>F6/1000</f>
+        <v>3.0499999999999998E-3</v>
+      </c>
+      <c r="F23" s="64">
+        <f>H6</f>
+        <v>1.0966666666666666E-2</v>
+      </c>
+      <c r="G23" s="67">
+        <f t="shared" si="5"/>
+        <v>1.3379333333333333E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E15:F15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0877AA7D-3E8E-462C-96DD-24C51B19A964}">
-  <dimension ref="B1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0877AA7D-3E8E-462C-96DD-24C51B19A964}">
+  <dimension ref="B1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3632,9 +3877,134 @@
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I13" s="61"/>
     </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G16" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="65"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G18" s="63">
+        <f>F12/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="64">
+        <f>H12</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I18" s="67">
+        <f>H18*$D$20</f>
+        <v>4.8799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="63">
+        <f>F11/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="64">
+        <f>H11</f>
+        <v>6.8888888888888884E-4</v>
+      </c>
+      <c r="I19" s="67">
+        <f t="shared" ref="I19:I24" si="5">H19*$D$20</f>
+        <v>8.4044444444444433E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="66">
+        <v>1.22</v>
+      </c>
+      <c r="G20" s="63">
+        <f>F10/1000</f>
+        <v>3.9999999999999996E-4</v>
+      </c>
+      <c r="H20" s="64">
+        <f>H10</f>
+        <v>6.8888888888888884E-4</v>
+      </c>
+      <c r="I20" s="67">
+        <f t="shared" si="5"/>
+        <v>8.4044444444444433E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G21" s="63">
+        <f>F9/1000</f>
+        <v>1.1300000000000001E-3</v>
+      </c>
+      <c r="H21" s="64">
+        <f>H9</f>
+        <v>1.1055555555555556E-3</v>
+      </c>
+      <c r="I21" s="67">
+        <f t="shared" si="5"/>
+        <v>1.3487777777777777E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G22" s="63">
+        <f>F8/1000</f>
+        <v>1.7033333333333334E-3</v>
+      </c>
+      <c r="H22" s="64">
+        <f>H8</f>
+        <v>1.3092592592592591E-3</v>
+      </c>
+      <c r="I22" s="67">
+        <f t="shared" si="5"/>
+        <v>1.5972962962962961E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="63">
+        <f>F7/1000</f>
+        <v>2.4599999999999999E-3</v>
+      </c>
+      <c r="H23" s="64">
+        <f>H7</f>
+        <v>1.4777777777777779E-3</v>
+      </c>
+      <c r="I23" s="67">
+        <f t="shared" si="5"/>
+        <v>1.802888888888889E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="63">
+        <f>F6/1000</f>
+        <v>3.3733333333333337E-3</v>
+      </c>
+      <c r="H24" s="64">
+        <f>H6</f>
+        <v>2.1481481481481482E-3</v>
+      </c>
+      <c r="I24" s="67">
+        <f t="shared" si="5"/>
+        <v>2.6207407407407408E-3</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G16:H16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>